<commit_message>
RayT_Math.h: Neu: header datei zu einem kommenden cpp implementierung.
RayT_Math wird mathematische formeln für die Ray berechnungen enthalten (.cpp folgt)

Zeiterfassung_Welsch_Dennis.xlsx: zeiterfassung

Zeiten nachgetragen. Ist nicht 100% genau durch lesen / forschungen im bus
</commit_message>
<xml_diff>
--- a/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Welsch_Dennis.xlsx
+++ b/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Welsch_Dennis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\FR1PEPF0000110C\EXCELCNV\38be13ca-7930-4907-bf57-2ec3b5eddf68\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwels\VSCODE\RaytRazor\1. Projektplanung\1.1 Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{AA14E6DE-C023-49F3-978B-FAACC8F95189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB8A500C-58E1-48E2-927A-060588CB57D3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6821C-D4A7-494C-90B8-EC34C17C17F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{13671DE0-EAD2-44F3-A1E0-C608E2EB2296}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{13671DE0-EAD2-44F3-A1E0-C608E2EB2296}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Name:</t>
   </si>
@@ -47,9 +47,6 @@
     <t>MatrNr:</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Projekt:</t>
   </si>
   <si>
@@ -75,13 +72,40 @@
   </si>
   <si>
     <t>Teilnahme am Kickoff-Meeting</t>
+  </si>
+  <si>
+    <t>Rayforge</t>
+  </si>
+  <si>
+    <t>1h 10min</t>
+  </si>
+  <si>
+    <t>Gruppe Kickoff-Meeting</t>
+  </si>
+  <si>
+    <t>Einarbeiten</t>
+  </si>
+  <si>
+    <t>Einlesen in Raytracing</t>
+  </si>
+  <si>
+    <t>Besprechung des Projekt umfangs</t>
+  </si>
+  <si>
+    <t>Notfall besprechung</t>
+  </si>
+  <si>
+    <t>Programmieren</t>
+  </si>
+  <si>
+    <t>Erstes konzept der Raytracer Math library</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -99,13 +123,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -136,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -151,10 +168,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -430,13 +450,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11EDF1B-A292-464D-9512-73DA35F01323}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="2" customWidth="1"/>
@@ -445,7 +465,7 @@
     <col min="5" max="256" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -453,67 +473,167 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7">
+        <v>3139911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>45574</v>
       </c>
       <c r="B7" s="2">
         <v>1.5</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>45579</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>45585</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>45586</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>45587</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>45592</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EA32FAADEF28B246BE81F09370D9BDD6" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee5e8cab159ec08823d71aeff920ea58">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcfc458b-b0e2-47b4-8909-d39697dfebcc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6553d0449cd115c0021964cc0df6b6b1" ns2:_="">
     <xsd:import namespace="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
@@ -657,29 +777,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C2E7B8-E028-453E-8691-C0FBD2FB7CE2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC5825A0-9928-4DC4-96F2-A5F9419A53C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7FC1F3-F6F1-4513-BD25-A27348CF4110}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7FC1F3-F6F1-4513-BD25-A27348CF4110}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC5825A0-9928-4DC4-96F2-A5F9419A53C9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C2E7B8-E028-453E-8691-C0FBD2FB7CE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>